<commit_message>
slight improvement, but known bug when reset at halftime: initial uncorrect countdown
</commit_message>
<xml_diff>
--- a/C5Team/Torneo2021.xlsx
+++ b/C5Team/Torneo2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leone\Desktop\Home\programmi_Python\GitTest\C5Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8623FBE-C23B-4AC2-B30E-DD9CCC5ED9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8C0D11-130F-47DC-9823-75BDCCDD575C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -475,14 +475,16 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -701,7 +703,7 @@
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -711,7 +713,7 @@
   <sheetData>
     <row r="1" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="39">
+      <c r="B2" s="38">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -741,7 +743,7 @@
       <c r="K2" s="2">
         <v>50</v>
       </c>
-      <c r="M2" s="37">
+      <c r="M2" s="40">
         <v>0</v>
       </c>
       <c r="N2" s="1" t="s">
@@ -773,7 +775,7 @@
       </c>
     </row>
     <row r="3" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="40"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
@@ -799,7 +801,7 @@
         <f t="shared" ref="L3:L9" si="0">IF(SUM(E3:K3)=4,"","ERRORE")</f>
         <v/>
       </c>
-      <c r="M3" s="38"/>
+      <c r="M3" s="41"/>
       <c r="N3" s="2" t="s">
         <v>2</v>
       </c>
@@ -827,7 +829,7 @@
       </c>
     </row>
     <row r="4" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="40"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -853,7 +855,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M4" s="38"/>
+      <c r="M4" s="41"/>
       <c r="N4" s="2" t="s">
         <v>4</v>
       </c>
@@ -881,7 +883,7 @@
       </c>
     </row>
     <row r="5" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="40"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -907,7 +909,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M5" s="38"/>
+      <c r="M5" s="41"/>
       <c r="N5" s="2" t="s">
         <v>6</v>
       </c>
@@ -935,7 +937,7 @@
       </c>
     </row>
     <row r="6" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="40"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
@@ -961,7 +963,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M6" s="38"/>
+      <c r="M6" s="41"/>
       <c r="N6" s="2" t="s">
         <v>10</v>
       </c>
@@ -989,7 +991,7 @@
       </c>
     </row>
     <row r="7" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="40"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1015,7 +1017,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M7" s="38"/>
+      <c r="M7" s="41"/>
       <c r="N7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1043,7 +1045,7 @@
       </c>
     </row>
     <row r="8" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1069,7 +1071,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M8" s="38"/>
+      <c r="M8" s="41"/>
       <c r="N8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1097,11 +1099,11 @@
       </c>
     </row>
     <row r="9" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="40"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="42" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="6"/>
@@ -1123,7 +1125,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M9" s="38"/>
+      <c r="M9" s="41"/>
       <c r="N9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1151,6 +1153,7 @@
       </c>
     </row>
     <row r="10" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="37"/>
       <c r="E10" s="2">
         <v>7</v>
       </c>
@@ -2885,7 +2888,7 @@
       <c r="A2" s="12">
         <v>6</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B2" s="40">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2922,7 +2925,7 @@
         <f>7*50/A2</f>
         <v>58.333333333333336</v>
       </c>
-      <c r="M2" s="37">
+      <c r="M2" s="40">
         <v>0</v>
       </c>
       <c r="N2" s="1" t="s">
@@ -2954,7 +2957,7 @@
       </c>
     </row>
     <row r="3" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="38"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2980,7 +2983,7 @@
         <f t="shared" ref="L3:L9" si="0">IF(SUM(E3:K3)=4,"","ERRORE")</f>
         <v/>
       </c>
-      <c r="M3" s="38"/>
+      <c r="M3" s="41"/>
       <c r="N3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3008,7 +3011,7 @@
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="38"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
@@ -3034,7 +3037,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M4" s="38"/>
+      <c r="M4" s="41"/>
       <c r="N4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3062,7 +3065,7 @@
       </c>
     </row>
     <row r="5" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="38"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -3088,7 +3091,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M5" s="38"/>
+      <c r="M5" s="41"/>
       <c r="N5" s="2" t="s">
         <v>6</v>
       </c>
@@ -3116,7 +3119,7 @@
       </c>
     </row>
     <row r="6" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="38"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
@@ -3142,7 +3145,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M6" s="38"/>
+      <c r="M6" s="41"/>
       <c r="N6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3170,7 +3173,7 @@
       </c>
     </row>
     <row r="7" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="38"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
@@ -3196,7 +3199,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M7" s="38"/>
+      <c r="M7" s="41"/>
       <c r="N7" s="2" t="s">
         <v>8</v>
       </c>
@@ -3224,7 +3227,7 @@
       </c>
     </row>
     <row r="8" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="38"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
@@ -3250,7 +3253,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M8" s="38"/>
+      <c r="M8" s="41"/>
       <c r="N8" s="2" t="s">
         <v>14</v>
       </c>
@@ -3278,7 +3281,7 @@
       </c>
     </row>
     <row r="9" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="38"/>
+      <c r="B9" s="41"/>
       <c r="E9" s="34"/>
       <c r="F9" s="34"/>
       <c r="G9" s="34"/>
@@ -3290,7 +3293,7 @@
         <f t="shared" si="0"/>
         <v>ERRORE</v>
       </c>
-      <c r="M9" s="38"/>
+      <c r="M9" s="41"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>

</xml_diff>